<commit_message>
updated pres, organized folders, add server side cursor
</commit_message>
<xml_diff>
--- a/ppt/riffle.xlsx
+++ b/ppt/riffle.xlsx
@@ -149,7 +149,9 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="C00000"/>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -251,7 +253,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -271,21 +272,13 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$D$2:$D$4</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Positive_x000d_(5 and 4 Stars)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Middle_x000d_(3 Stars)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Negative_x000d_(1 and 2 Stars)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -315,11 +308,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="107"/>
-        <c:axId val="-1721604912"/>
-        <c:axId val="-1721325360"/>
+        <c:axId val="-342807040"/>
+        <c:axId val="-343381072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1721604912"/>
+        <c:axId val="-342807040"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -359,7 +352,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1721325360"/>
+        <c:crossAx val="-343381072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -367,7 +360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1721325360"/>
+        <c:axId val="-343381072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +369,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1721604912"/>
+        <c:crossAx val="-342807040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -974,13 +967,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1268,7 +1261,7 @@
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1276,16 +1269,17 @@
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5</v>
       </c>
       <c r="B2">
         <v>1704200</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="3"/>
       <c r="E2">
         <f>SUM(B2:B3)</f>
         <v>2736854</v>
@@ -1302,9 +1296,10 @@
       <c r="B3">
         <v>1032654</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="3"/>
       <c r="E3">
         <f>B4</f>
         <v>517369</v>
@@ -1314,16 +1309,17 @@
         <v>0.12457267375365687</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>517369</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="1">
         <f>SUM(B5:B6)</f>
         <v>898927</v>

</xml_diff>